<commit_message>
Store Card Function Enabled.
</commit_message>
<xml_diff>
--- a/Mall.xlsx
+++ b/Mall.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21580" windowHeight="9500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7880" yWindow="460" windowWidth="21580" windowHeight="9500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NEW MALL" sheetId="3" r:id="rId1"/>
@@ -146,7 +146,157 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1494,32 +1644,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:V1 A4:V4 A2:A3 D2:D3 I2:V3 L7:O8 A9:O9 A5:A8 A10:A11 M10:O10 D10:D11 D5:D8 I5:O6 I7:I8 I10:K10 I11:J11 Q5:V10 Q11 A12:P12 R12">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="6" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A12">
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12 V11:V12">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T12:U12">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11:U11">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q12">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1533,13 +1683,13 @@
   <dimension ref="A1:V264"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="22" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="22" width="3.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -1680,19 +1830,19 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>802</v>
+        <v>999</v>
       </c>
       <c r="B3">
-        <v>802</v>
+        <v>999</v>
       </c>
       <c r="C3">
-        <v>802</v>
+        <v>999</v>
       </c>
       <c r="D3">
-        <v>802</v>
+        <v>999</v>
       </c>
       <c r="E3">
-        <v>999</v>
+        <v>811</v>
       </c>
       <c r="F3">
         <v>101</v>
@@ -1748,16 +1898,16 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>803</v>
+        <v>999</v>
       </c>
       <c r="B4">
-        <v>803</v>
+        <v>999</v>
       </c>
       <c r="C4">
-        <v>803</v>
+        <v>999</v>
       </c>
       <c r="D4">
-        <v>803</v>
+        <v>999</v>
       </c>
       <c r="E4">
         <v>999</v>
@@ -1816,19 +1966,19 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>804</v>
+        <v>812</v>
       </c>
       <c r="B5">
-        <v>804</v>
+        <v>812</v>
       </c>
       <c r="C5">
-        <v>804</v>
+        <v>812</v>
       </c>
       <c r="D5">
-        <v>804</v>
+        <v>812</v>
       </c>
       <c r="E5">
-        <v>999</v>
+        <v>812</v>
       </c>
       <c r="F5">
         <v>102</v>
@@ -1884,19 +2034,19 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>999</v>
+        <v>813</v>
       </c>
       <c r="B6">
-        <v>999</v>
+        <v>813</v>
       </c>
       <c r="C6">
-        <v>999</v>
+        <v>813</v>
       </c>
       <c r="D6">
-        <v>999</v>
+        <v>813</v>
       </c>
       <c r="E6">
-        <v>999</v>
+        <v>813</v>
       </c>
       <c r="F6">
         <v>102</v>
@@ -2373,25 +2523,25 @@
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>802</v>
+        <v>999</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>803</v>
+        <v>999</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>804</v>
+        <v>812</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>999</v>
+        <v>813</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -2445,25 +2595,25 @@
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="1"/>
-        <v>802</v>
+        <v>999</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="1"/>
-        <v>803</v>
+        <v>999</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="1"/>
-        <v>804</v>
+        <v>812</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="1"/>
-        <v>999</v>
+        <v>813</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
@@ -2517,25 +2667,25 @@
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="2"/>
-        <v>802</v>
+        <v>999</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="2"/>
-        <v>803</v>
+        <v>999</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="2"/>
-        <v>804</v>
+        <v>812</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="2"/>
-        <v>999</v>
+        <v>813</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
@@ -2589,7 +2739,7 @@
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="3"/>
-        <v>999</v>
+        <v>811</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
@@ -2601,13 +2751,13 @@
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="3"/>
-        <v>999</v>
+        <v>812</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="3"/>
-        <v>999</v>
+        <v>813</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
@@ -3871,77 +4021,122 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V6 F12:P12 T1:V5 B1:D5 V12 T7:V11 F1:S1 G2:H3 O7:S8 G10:H11 G5:H8 L5:S6 L7:M8 M10:S10 L10:N11 L2:T3 F9:S9 F4:T4">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+  <conditionalFormatting sqref="V6 F12:P12 T1:V5 B1:D2 V12 T7:V11 F1:S1 G2:H3 O7:S8 G10:H11 G5:H8 L5:S6 L7:M8 M10:S10 L10:N11 L2:T3 F9:S9 F4:T4">
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A264">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6:U6 T12:U12">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="24" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:D6">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11 B7:D10">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="20" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q12:S17">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A5">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+  <conditionalFormatting sqref="A1:A2">
+    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A10 A12">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D12">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+      <formula>999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E2 E7:E11">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+      <formula>999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6 E12">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+      <formula>999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:D5">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+      <formula>999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+      <formula>999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:D4">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:D3">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E5 E7:E11">
+  <conditionalFormatting sqref="A3">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6 E12">
+  <conditionalFormatting sqref="E3">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>999</formula>
     </cfRule>

</xml_diff>

<commit_message>
TBH IDK what changed.
</commit_message>
<xml_diff>
--- a/Mall.xlsx
+++ b/Mall.xlsx
@@ -5350,8 +5350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
U may need to fix this lol
</commit_message>
<xml_diff>
--- a/Mall.xlsx
+++ b/Mall.xlsx
@@ -5350,8 +5350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>